<commit_message>
Hashmap program updated and timesheet added
</commit_message>
<xml_diff>
--- a/Madan/Timesheet/Schwall_TraineeName_Timesheet_June_2021.xlsx
+++ b/Madan/Timesheet/Schwall_TraineeName_Timesheet_June_2021.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B9E506-FFE1-4B35-84E0-C2F0FE81F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8045FB41-05B0-4CA5-B8E3-EFFE4958AA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>SlNo</t>
   </si>
@@ -114,6 +114,27 @@
   </si>
   <si>
     <t>4hrs</t>
+  </si>
+  <si>
+    <t>Hashmap,HashTable concepts and eclipse functions</t>
+  </si>
+  <si>
+    <t>21/2hrs</t>
+  </si>
+  <si>
+    <t>Hashtable program</t>
+  </si>
+  <si>
+    <t>program using hashmap for insert,search,update,remove values</t>
+  </si>
+  <si>
+    <t>31/2 hrs</t>
+  </si>
+  <si>
+    <t>5hrs</t>
+  </si>
+  <si>
+    <t>Revised the training period learned concepts and also previous class learned topics</t>
   </si>
 </sst>
 </file>
@@ -616,7 +637,7 @@
   <dimension ref="B1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,25 +814,47 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10">
+        <v>44355</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="3"/>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="2"/>

</xml_diff>

<commit_message>
Timesheet and program task updated
</commit_message>
<xml_diff>
--- a/Madan/Timesheet/Schwall_TraineeName_Timesheet_June_2021.xlsx
+++ b/Madan/Timesheet/Schwall_TraineeName_Timesheet_June_2021.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6CBAD5-760D-49A7-99D4-1FA1FC8AEFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C60E6D-FBAA-45B9-9DF8-3EA7DCF3D789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,12 +263,6 @@
     <t>30 mins</t>
   </si>
   <si>
-    <t>jbpm task</t>
-  </si>
-  <si>
-    <t>created a sample project by using jbpm concepts</t>
-  </si>
-  <si>
     <t xml:space="preserve">Revised the java collections </t>
   </si>
   <si>
@@ -312,6 +306,12 @@
   </si>
   <si>
     <t>Maven concepts and about how to import project and download the project in jbpm.And about its setting configuration.</t>
+  </si>
+  <si>
+    <t>jbpm task, Java Task</t>
+  </si>
+  <si>
+    <t>created a sample project by using jbpm concepts, created a program using arraylist for string type using length</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
   <dimension ref="B1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1420,10 +1420,10 @@
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>18</v>
@@ -1440,7 +1440,7 @@
         <v>16</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>36</v>
@@ -1450,10 +1450,10 @@
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>30</v>
@@ -1463,13 +1463,13 @@
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.35">
@@ -1480,10 +1480,10 @@
         <v>44368</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>36</v>
@@ -1493,10 +1493,10 @@
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>30</v>
@@ -1506,13 +1506,13 @@
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.35">
@@ -1526,7 +1526,7 @@
         <v>22</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>67</v>
@@ -1536,10 +1536,10 @@
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>50</v>

</xml_diff>